<commit_message>
MAINTENANCE Update Pair Matrix
</commit_message>
<xml_diff>
--- a/PairProgramming/PairingMatirx_Team_01.xlsx
+++ b/PairProgramming/PairingMatirx_Team_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignaz.oetzlinger\StudioProjects\Team_01\PairProgramming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijoet\Documents\Team_01\PairProgramming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBD0CD1-7EAC-4EBF-9C36-804C2DE3E75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C3B20C-E345-4742-82A4-B1035F07F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,20 +492,20 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" style="13" customWidth="1"/>
-    <col min="9" max="10" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="13" customWidth="1"/>
+    <col min="9" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -517,7 +517,7 @@
       <c r="G1" s="15"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="str">
         <f>A3</f>
         <v>Felix Schmidt</v>
@@ -546,7 +546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -562,7 +562,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -578,7 +578,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -594,7 +594,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -615,7 +615,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -639,7 +639,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -666,7 +666,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -692,7 +692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -725,10 +725,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>2</v>
       </c>
@@ -740,7 +740,7 @@
       <c r="G12" s="15"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="str">
         <f>A14</f>
         <v>Felix Schmidt</v>
@@ -770,7 +770,7 @@
         <v>Florian Buchacher</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -782,12 +782,12 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -801,7 +801,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -813,13 +813,13 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -831,19 +831,19 @@
         <v>0</v>
       </c>
       <c r="D17" s="5">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="5">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5">
@@ -859,7 +859,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -885,10 +885,10 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="4">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -906,110 +906,110 @@
         <v>0</v>
       </c>
       <c r="G20" s="5">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="8">
-        <f>SUM(B14:B20)</f>
-        <v>240</v>
+        <f t="shared" ref="B21:H21" si="2">SUM(B14:B20)</f>
+        <v>330</v>
       </c>
       <c r="C21" s="8">
-        <f>SUM(C14:C20)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D21" s="8">
-        <f>SUM(D14:D20)</f>
-        <v>240</v>
+        <f t="shared" si="2"/>
+        <v>330</v>
       </c>
       <c r="E21" s="8">
-        <f>SUM(E14:E20)</f>
-        <v>240</v>
+        <f t="shared" si="2"/>
+        <v>330</v>
       </c>
       <c r="F21" s="8">
-        <f>SUM(F14:F20)</f>
-        <v>240</v>
+        <f t="shared" si="2"/>
+        <v>330</v>
       </c>
       <c r="G21" s="8">
-        <f>SUM(G14:G20)</f>
-        <v>240</v>
+        <f t="shared" si="2"/>
+        <v>330</v>
       </c>
       <c r="H21" s="8">
-        <f>SUM(H14:H20)</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="10">
-        <f t="shared" ref="B23:G23" si="2">B10+B21</f>
-        <v>240</v>
+        <f t="shared" ref="B23:G23" si="3">B10+B21</f>
+        <v>330</v>
       </c>
       <c r="C23" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D23" s="10">
-        <f t="shared" si="2"/>
-        <v>240</v>
+        <f t="shared" si="3"/>
+        <v>330</v>
       </c>
       <c r="E23" s="10">
-        <f t="shared" si="2"/>
-        <v>240</v>
+        <f t="shared" si="3"/>
+        <v>330</v>
       </c>
       <c r="F23" s="10">
-        <f t="shared" si="2"/>
-        <v>240</v>
+        <f t="shared" si="3"/>
+        <v>330</v>
       </c>
       <c r="G23" s="10">
-        <f t="shared" si="2"/>
-        <v>240</v>
+        <f t="shared" si="3"/>
+        <v>330</v>
       </c>
       <c r="H23" s="10">
-        <f t="shared" ref="H23" si="3">H10+H21</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H23" si="4">H10+H21</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="12">
-        <f t="shared" ref="B24:G24" si="4">B23/60/24</f>
-        <v>0.16666666666666666</v>
+        <f t="shared" ref="B24:G24" si="5">B23/60/24</f>
+        <v>0.22916666666666666</v>
       </c>
       <c r="C24" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D24" s="12">
-        <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <f t="shared" si="5"/>
+        <v>0.22916666666666666</v>
       </c>
       <c r="E24" s="12">
-        <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <f t="shared" si="5"/>
+        <v>0.22916666666666666</v>
       </c>
       <c r="F24" s="12">
-        <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <f t="shared" si="5"/>
+        <v>0.22916666666666666</v>
       </c>
       <c r="G24" s="12">
-        <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <f t="shared" si="5"/>
+        <v>0.22916666666666666</v>
       </c>
       <c r="H24" s="12">
-        <f t="shared" ref="H24" si="5">H23/60/24</f>
-        <v>0.16666666666666666</v>
+        <f t="shared" ref="H24" si="6">H23/60/24</f>
+        <v>0.22916666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAINTENANCE Update Pair Matrix [IÖ]
</commit_message>
<xml_diff>
--- a/PairProgramming/PairingMatirx_Team_01.xlsx
+++ b/PairProgramming/PairingMatirx_Team_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijoet\Documents\Team_01\PairProgramming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignaz.oetzlinger\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C3B20C-E345-4742-82A4-B1035F07F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AB0BC0B-10DC-43EF-84EC-1A76B7D3A83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Number of minutes the two members did physically co-located ping pong pair programming.</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Florian Buchacher</t>
-  </si>
-  <si>
-    <t>3rd Observer Ermal</t>
   </si>
 </sst>
 </file>
@@ -492,7 +489,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -774,15 +771,13 @@
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B14" s="3"/>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4">
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -791,7 +786,10 @@
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5">
+        <f>C14</f>
+        <v>0</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15">
         <v>0</v>
@@ -806,14 +804,16 @@
         <v>7</v>
       </c>
       <c r="B16" s="5">
+        <f>D14</f>
         <v>0</v>
       </c>
       <c r="C16" s="5">
+        <f>D15</f>
         <v>0</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -824,6 +824,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="5">
+        <f>E14</f>
         <v>0</v>
       </c>
       <c r="C17" s="5">
@@ -831,7 +832,8 @@
         <v>0</v>
       </c>
       <c r="D17" s="5">
-        <v>330</v>
+        <f>E16</f>
+        <v>360</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
@@ -843,19 +845,22 @@
         <v>9</v>
       </c>
       <c r="B18" s="5">
-        <v>330</v>
-      </c>
-      <c r="C18" s="5"/>
+        <f>F14</f>
+        <v>240</v>
+      </c>
+      <c r="C18" s="5">
+        <f>F15</f>
+        <v>0</v>
+      </c>
       <c r="D18" s="5">
         <f>F16</f>
         <v>0</v>
       </c>
       <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>12</v>
-      </c>
+        <f>E17</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
@@ -885,28 +890,35 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="4">
-        <v>330</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="5">
+        <f>H14</f>
+        <v>0</v>
+      </c>
       <c r="C20" s="5">
+        <f>H15</f>
         <v>0</v>
       </c>
       <c r="D20" s="5">
+        <f>H16</f>
         <v>0</v>
       </c>
       <c r="E20" s="5">
+        <f>H17</f>
         <v>0</v>
       </c>
       <c r="F20" s="5">
+        <f>H18</f>
         <v>0</v>
       </c>
       <c r="G20" s="5">
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="H20" s="3"/>
     </row>
@@ -916,7 +928,7 @@
       </c>
       <c r="B21" s="8">
         <f t="shared" ref="B21:H21" si="2">SUM(B14:B20)</f>
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="C21" s="8">
         <f t="shared" si="2"/>
@@ -924,23 +936,23 @@
       </c>
       <c r="D21" s="8">
         <f t="shared" si="2"/>
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="E21" s="8">
         <f t="shared" si="2"/>
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="F21" s="8">
         <f t="shared" si="2"/>
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="G21" s="8">
         <f t="shared" si="2"/>
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="H21" s="8">
         <f t="shared" si="2"/>
-        <v>330</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -952,7 +964,7 @@
       </c>
       <c r="B23" s="10">
         <f t="shared" ref="B23:G23" si="3">B10+B21</f>
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="C23" s="10">
         <f t="shared" si="3"/>
@@ -960,23 +972,23 @@
       </c>
       <c r="D23" s="10">
         <f t="shared" si="3"/>
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="E23" s="10">
         <f t="shared" si="3"/>
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="F23" s="10">
         <f t="shared" si="3"/>
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="G23" s="10">
         <f t="shared" si="3"/>
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="H23" s="10">
         <f t="shared" ref="H23" si="4">H10+H21</f>
-        <v>330</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -985,7 +997,7 @@
       </c>
       <c r="B24" s="12">
         <f t="shared" ref="B24:G24" si="5">B23/60/24</f>
-        <v>0.22916666666666666</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C24" s="12">
         <f t="shared" si="5"/>
@@ -993,23 +1005,23 @@
       </c>
       <c r="D24" s="12">
         <f t="shared" si="5"/>
-        <v>0.22916666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="E24" s="12">
         <f t="shared" si="5"/>
-        <v>0.22916666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="5"/>
-        <v>0.22916666666666666</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G24" s="12">
         <f t="shared" si="5"/>
-        <v>0.22916666666666666</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H24" s="12">
         <f t="shared" ref="H24" si="6">H23/60/24</f>
-        <v>0.22916666666666666</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>